<commit_message>
ya subi excel de colaboradores
</commit_message>
<xml_diff>
--- a/subidas/usuarios.xlsx
+++ b/subidas/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gvillanuevap\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB01AFC-B477-4AF6-9B84-79F47F639234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9615857-06B9-4495-A247-9CC1927BD37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4820" yWindow="4820" windowWidth="28800" windowHeight="15460" xr2:uid="{A6294EFB-B2FC-48BE-8E32-3281D1B8E2D8}"/>
   </bookViews>
@@ -36,17 +36,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
   <si>
-    <t>NOMBRE DEL COLABORADOR DESDE BD</t>
+    <t>peroos</t>
+  </si>
+  <si>
+    <t>INICIO</t>
+  </si>
+  <si>
+    <t>FIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -74,8 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA00CBAA-1361-463D-80EA-CAEF2D0FC5A4}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -401,9 +416,9 @@
     <col min="1" max="1" width="34.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1">
         <v>65799</v>
@@ -411,8 +426,134 @@
       <c r="C1">
         <v>123456</v>
       </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>65799</v>
+      </c>
+      <c r="C2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>65799</v>
+      </c>
+      <c r="C3">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>65799</v>
+      </c>
+      <c r="C4">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>65799</v>
+      </c>
+      <c r="C5">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>65799</v>
+      </c>
+      <c r="C6">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>65799</v>
+      </c>
+      <c r="C7">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>65799</v>
+      </c>
+      <c r="C8">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>65799</v>
+      </c>
+      <c r="C9">
+        <v>123456</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>65799</v>
+      </c>
+      <c r="C10">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>65799</v>
+      </c>
+      <c r="C11">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>65799</v>
+      </c>
+      <c r="C12">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ya sube colanoradors desde csv
</commit_message>
<xml_diff>
--- a/subidas/usuarios.xlsx
+++ b/subidas/usuarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gvillanuevap\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9615857-06B9-4495-A247-9CC1927BD37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45D3E00-52EF-42A9-B297-D050AB2971C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="4820" windowWidth="28800" windowHeight="15460" xr2:uid="{A6294EFB-B2FC-48BE-8E32-3281D1B8E2D8}"/>
+    <workbookView xWindow="1350" yWindow="2030" windowWidth="28800" windowHeight="15460" xr2:uid="{A6294EFB-B2FC-48BE-8E32-3281D1B8E2D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
-    <t>peroos</t>
+    <t>Número Nomina</t>
   </si>
   <si>
-    <t>INICIO</t>
+    <t>Password</t>
   </si>
   <si>
-    <t>FIN</t>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>68657</t>
+  </si>
+  <si>
+    <t>inicio</t>
+  </si>
+  <si>
+    <t>fin</t>
   </si>
 </sst>
 </file>
@@ -60,7 +69,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -88,9 +97,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,152 +419,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA00CBAA-1361-463D-80EA-CAEF2D0FC5A4}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.08984375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>65799</v>
-      </c>
-      <c r="C1">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>65799</v>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C2">
         <v>123456</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>65799</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C3">
         <v>123456</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>65799</v>
-      </c>
-      <c r="C4">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>65799</v>
-      </c>
-      <c r="C5">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>65799</v>
-      </c>
-      <c r="C6">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>65799</v>
-      </c>
-      <c r="C7">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>65799</v>
-      </c>
-      <c r="C8">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>65799</v>
-      </c>
-      <c r="C9">
-        <v>123456</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>65799</v>
-      </c>
-      <c r="C10">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>65799</v>
-      </c>
-      <c r="C11">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>65799</v>
-      </c>
-      <c r="C12">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E16" s="1"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>